<commit_message>
Added cover sheet to excel workbook
</commit_message>
<xml_diff>
--- a/data/infl_unempl.xlsx
+++ b/data/infl_unempl.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e7bb2393f2f09c0/Documents/RProjects/infl_v_unemp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{8101EAF8-B27A-43A2-870A-D3C81822AC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{931D2213-2F63-4E0C-89E7-EE9C10088D4A}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="8_{8101EAF8-B27A-43A2-870A-D3C81822AC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0770F37-614A-4DF7-AA45-B293EEB51590}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="8856" yWindow="4656" windowWidth="19620" windowHeight="12264" xr2:uid="{A34EDC3C-D948-4C0A-862C-029CA38B8FA9}"/>
+    <workbookView xWindow="9204" yWindow="5004" windowWidth="19620" windowHeight="12264" xr2:uid="{A34EDC3C-D948-4C0A-862C-029CA38B8FA9}"/>
   </bookViews>
   <sheets>
-    <sheet name="CPIAUCSL" sheetId="1" r:id="rId1"/>
-    <sheet name="UNRATE" sheetId="5" r:id="rId2"/>
+    <sheet name="CoverSheet" sheetId="6" r:id="rId1"/>
+    <sheet name="CPIAUCSL" sheetId="1" r:id="rId2"/>
+    <sheet name="UNRATE" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>CPIAUCSL</t>
   </si>
@@ -76,6 +78,33 @@
   <si>
     <t>1948-01-01 to 2022-03-01</t>
   </si>
+  <si>
+    <t xml:space="preserve">"The FRED Add-in provides free access to over 810,000 data series from various </t>
+  </si>
+  <si>
+    <t>sources (e.g., BEA, BLS, Census, and OECD) directly through Microsoft Excel."</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/fred-addin/</t>
+  </si>
+  <si>
+    <t>This Excel workbook uses the FRED plug-in/extension to search, locate,</t>
+  </si>
+  <si>
+    <t>Once the data is loaded to a worksheet, it is exported in "csv" format and</t>
+  </si>
+  <si>
+    <t>all further processing and transformation is performed in R.</t>
+  </si>
+  <si>
+    <t>Get it!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and download un employment and CPI data from the ST Louis FED.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From their website: </t>
+  </si>
 </sst>
 </file>
 
@@ -85,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -96,6 +125,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -121,11 +156,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -142,6 +181,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>412152</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>122031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2EA19E7-13E9-E7ED-73EA-D461846E9745}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="586740" y="1691640"/>
+          <a:ext cx="7750212" cy="1280271"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,10 +528,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF256E87-1125-4FBF-87CA-E90CE85E39CE}">
+  <dimension ref="B3:C21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" xr:uid="{71CEF892-21BC-42D1-8C38-14A2FBCA43AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FFA661-BA9F-4FE7-8EF3-F90B0D1FC8D7}">
   <dimension ref="A1:B910"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7730,7 +7881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FCC18C-4435-45A0-898C-DC7FC35594CC}">
   <dimension ref="A1:B898"/>
   <sheetViews>

</xml_diff>